<commit_message>
fix spice latch circuit, started routing
</commit_message>
<xml_diff>
--- a/hardware/tl494-BOM.xlsx
+++ b/hardware/tl494-BOM.xlsx
@@ -15,8 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$46</definedName>
-    <definedName name="tl494_" localSheetId="0">Sheet1!$A$1:$H$46</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$47</definedName>
+    <definedName name="tl494_" localSheetId="0">Sheet1!$A$1:$H$47</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="149">
   <si>
     <t>Qty</t>
   </si>
@@ -145,9 +145,6 @@
     <t>E3,5-10</t>
   </si>
   <si>
-    <t>C10, C11, C12</t>
-  </si>
-  <si>
     <t>POLARIZED CAPACITOR, European symbol</t>
   </si>
   <si>
@@ -488,6 +485,15 @@
   </si>
   <si>
     <t>330R</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>C10, C11</t>
+  </si>
+  <si>
+    <t>1000uF 63V</t>
   </si>
 </sst>
 </file>
@@ -834,10 +840,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -895,7 +901,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
@@ -915,7 +921,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
@@ -975,7 +981,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -1012,7 +1018,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>29</v>
@@ -1024,87 +1030,80 @@
         <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" t="s">
         <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>135</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -1112,59 +1111,59 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F15" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
@@ -1172,22 +1171,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1195,39 +1194,39 @@
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="F18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1235,19 +1234,19 @@
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>63</v>
+        <v>30</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F20" t="s">
-        <v>65</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1255,19 +1254,19 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F21" t="s">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1275,16 +1274,16 @@
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F22" t="s">
         <v>16</v>
@@ -1295,16 +1294,16 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F23" t="s">
         <v>16</v>
@@ -1315,19 +1314,19 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F24" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1335,19 +1334,19 @@
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="F25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1355,53 +1354,53 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>143</v>
+        <v>76</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
+      </c>
+      <c r="F26" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>82</v>
+        <v>142</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F27" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F28" t="s">
         <v>16</v>
@@ -1409,19 +1408,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E29" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F29" t="s">
         <v>16</v>
@@ -1429,19 +1428,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C30" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F30" t="s">
         <v>16</v>
@@ -1452,16 +1451,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E31" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F31" t="s">
         <v>16</v>
@@ -1472,16 +1471,16 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>94</v>
+        <v>35</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F32" t="s">
         <v>16</v>
@@ -1489,19 +1488,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>36</v>
+        <v>93</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F33" t="s">
         <v>16</v>
@@ -1509,19 +1508,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F34" t="s">
         <v>16</v>
@@ -1532,16 +1531,16 @@
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>145</v>
+        <v>97</v>
       </c>
       <c r="C35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F35" t="s">
         <v>16</v>
@@ -1552,19 +1551,19 @@
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>102</v>
+        <v>34</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>103</v>
+        <v>35</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F36" t="s">
-        <v>105</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,19 +1571,19 @@
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>35</v>
+        <v>101</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>36</v>
+        <v>102</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F37" t="s">
-        <v>16</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1592,16 +1591,16 @@
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F38" t="s">
         <v>16</v>
@@ -1609,102 +1608,102 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F39" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
         <v>2</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="B42" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="2" t="s">
+      <c r="E42" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F41" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>1</v>
-      </c>
-      <c r="B42" s="2" t="s">
+      <c r="C43" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F43" t="s">
         <v>116</v>
-      </c>
-      <c r="F42" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>1</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F43" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1712,56 +1711,76 @@
         <v>1</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="F44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F45" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>1</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>1</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="F44" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
-        <v>1</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E45" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
-        <v>1</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="2" t="s">
+      <c r="D47" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F47" t="s">
         <v>130</v>
-      </c>
-      <c r="F46" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>